<commit_message>
add model inference time estimation
</commit_message>
<xml_diff>
--- a/simplecnn_profile.xlsx
+++ b/simplecnn_profile.xlsx
@@ -428,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H16"/>
+  <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -436,7 +436,7 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="32" customWidth="1" min="1" max="1"/>
+    <col width="27" customWidth="1" min="1" max="1"/>
     <col width="17" customWidth="1" min="2" max="2"/>
     <col width="17" customWidth="1" min="3" max="3"/>
     <col width="11" customWidth="1" min="4" max="4"/>
@@ -523,94 +523,94 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="2" t="inlineStr">
-        <is>
-          <t>conv1.1 (BatchNorm2d)</t>
-        </is>
-      </c>
-      <c r="B3" s="2" t="inlineStr">
+      <c r="A3" s="1" t="inlineStr">
+        <is>
+          <t>conv2.0 (Conv2d)</t>
+        </is>
+      </c>
+      <c r="B3" s="1" t="inlineStr">
         <is>
           <t>(1, 16, 32, 32)</t>
         </is>
       </c>
-      <c r="C3" s="2" t="inlineStr">
-        <is>
-          <t>(1, 16, 32, 32)</t>
-        </is>
-      </c>
-      <c r="D3" s="2" t="n">
-        <v>0.032768</v>
-      </c>
-      <c r="E3" s="2" t="n">
-        <v>128.125</v>
-      </c>
-      <c r="F3" s="2" t="n">
-        <v>0.25</v>
-      </c>
-      <c r="G3" s="2" t="n">
-        <v>0.032</v>
-      </c>
-      <c r="H3" s="2" t="inlineStr">
-        <is>
-          <t>Memory-bound ❗</t>
+      <c r="C3" s="1" t="inlineStr">
+        <is>
+          <t>(1, 32, 16, 16)</t>
+        </is>
+      </c>
+      <c r="D3" s="1" t="n">
+        <v>9.437184</v>
+      </c>
+      <c r="E3" s="1" t="n">
+        <v>114.125</v>
+      </c>
+      <c r="F3" s="1" t="n">
+        <v>80.75</v>
+      </c>
+      <c r="G3" s="1" t="n">
+        <v>4.64</v>
+      </c>
+      <c r="H3" s="1" t="inlineStr">
+        <is>
+          <t>Balanced</t>
         </is>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="2" t="inlineStr">
-        <is>
-          <t>conv1.2 (ReLU)</t>
-        </is>
-      </c>
-      <c r="B4" s="2" t="inlineStr">
-        <is>
-          <t>(1, 16, 32, 32)</t>
-        </is>
-      </c>
-      <c r="C4" s="2" t="inlineStr">
-        <is>
-          <t>(1, 16, 32, 32)</t>
-        </is>
-      </c>
-      <c r="D4" s="2" t="n">
-        <v>0.016384</v>
-      </c>
-      <c r="E4" s="2" t="n">
-        <v>128</v>
-      </c>
-      <c r="F4" s="2" t="n">
-        <v>0.12</v>
-      </c>
-      <c r="G4" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="H4" s="2" t="inlineStr">
-        <is>
-          <t>Memory-bound ❗</t>
+      <c r="A4" s="1" t="inlineStr">
+        <is>
+          <t>conv3.cba_unit.0 (Conv2d)</t>
+        </is>
+      </c>
+      <c r="B4" s="1" t="inlineStr">
+        <is>
+          <t>(1, 32, 16, 16)</t>
+        </is>
+      </c>
+      <c r="C4" s="1" t="inlineStr">
+        <is>
+          <t>(1, 64, 8, 8)</t>
+        </is>
+      </c>
+      <c r="D4" s="1" t="n">
+        <v>9.437184</v>
+      </c>
+      <c r="E4" s="1" t="n">
+        <v>120</v>
+      </c>
+      <c r="F4" s="1" t="n">
+        <v>76.8</v>
+      </c>
+      <c r="G4" s="1" t="n">
+        <v>18.432</v>
+      </c>
+      <c r="H4" s="1" t="inlineStr">
+        <is>
+          <t>Balanced</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="2" t="inlineStr">
         <is>
-          <t>conv1 (Sequential)</t>
+          <t>conv3 (CBA)</t>
         </is>
       </c>
       <c r="B5" s="2" t="inlineStr">
         <is>
-          <t>(1, 3, 32, 32)</t>
+          <t>(1, 32, 16, 16)</t>
         </is>
       </c>
       <c r="C5" s="2" t="inlineStr">
         <is>
-          <t>(1, 16, 32, 32)</t>
+          <t>(1, 64, 8, 8)</t>
         </is>
       </c>
       <c r="D5" s="2" t="n">
         <v>0</v>
       </c>
       <c r="E5" s="2" t="n">
-        <v>76</v>
+        <v>48</v>
       </c>
       <c r="F5" s="2" t="n">
         <v>0</v>
@@ -625,374 +625,68 @@
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="1" t="inlineStr">
-        <is>
-          <t>conv2.0 (Conv2d)</t>
-        </is>
-      </c>
-      <c r="B6" s="1" t="inlineStr">
-        <is>
-          <t>(1, 16, 32, 32)</t>
-        </is>
-      </c>
-      <c r="C6" s="1" t="inlineStr">
-        <is>
-          <t>(1, 32, 16, 16)</t>
-        </is>
-      </c>
-      <c r="D6" s="1" t="n">
-        <v>9.437184</v>
-      </c>
-      <c r="E6" s="1" t="n">
-        <v>114.125</v>
-      </c>
-      <c r="F6" s="1" t="n">
-        <v>80.75</v>
-      </c>
-      <c r="G6" s="1" t="n">
-        <v>4.64</v>
-      </c>
-      <c r="H6" s="1" t="inlineStr">
-        <is>
-          <t>Balanced</t>
+      <c r="A6" s="2" t="inlineStr">
+        <is>
+          <t>fc (Linear)</t>
+        </is>
+      </c>
+      <c r="B6" s="2" t="inlineStr">
+        <is>
+          <t>(1, 4096)</t>
+        </is>
+      </c>
+      <c r="C6" s="2" t="inlineStr">
+        <is>
+          <t>(1, 10)</t>
+        </is>
+      </c>
+      <c r="D6" s="2" t="n">
+        <v>0.08192000000000001</v>
+      </c>
+      <c r="E6" s="2" t="n">
+        <v>176.078125</v>
+      </c>
+      <c r="F6" s="2" t="n">
+        <v>0.45</v>
+      </c>
+      <c r="G6" s="2" t="n">
+        <v>40.97</v>
+      </c>
+      <c r="H6" s="2" t="inlineStr">
+        <is>
+          <t>Memory-bound ❗</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="2" t="inlineStr">
         <is>
-          <t>conv2.1 (BatchNorm2d)</t>
+          <t xml:space="preserve"> (SimpleCNN)</t>
         </is>
       </c>
       <c r="B7" s="2" t="inlineStr">
         <is>
-          <t>(1, 32, 16, 16)</t>
+          <t>(1, 3, 32, 32)</t>
         </is>
       </c>
       <c r="C7" s="2" t="inlineStr">
         <is>
-          <t>(1, 32, 16, 16)</t>
+          <t>(1, 10)</t>
         </is>
       </c>
       <c r="D7" s="2" t="n">
-        <v>0.016384</v>
+        <v>0</v>
       </c>
       <c r="E7" s="2" t="n">
-        <v>64.25</v>
+        <v>12.0390625</v>
       </c>
       <c r="F7" s="2" t="n">
-        <v>0.25</v>
+        <v>0</v>
       </c>
       <c r="G7" s="2" t="n">
-        <v>0.064</v>
+        <v>0</v>
       </c>
       <c r="H7" s="2" t="inlineStr">
-        <is>
-          <t>Memory-bound ❗</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" s="2" t="inlineStr">
-        <is>
-          <t>conv2.2 (ReLU)</t>
-        </is>
-      </c>
-      <c r="B8" s="2" t="inlineStr">
-        <is>
-          <t>(1, 32, 16, 16)</t>
-        </is>
-      </c>
-      <c r="C8" s="2" t="inlineStr">
-        <is>
-          <t>(1, 32, 16, 16)</t>
-        </is>
-      </c>
-      <c r="D8" s="2" t="n">
-        <v>0.008192</v>
-      </c>
-      <c r="E8" s="2" t="n">
-        <v>64</v>
-      </c>
-      <c r="F8" s="2" t="n">
-        <v>0.12</v>
-      </c>
-      <c r="G8" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="H8" s="2" t="inlineStr">
-        <is>
-          <t>Memory-bound ❗</t>
-        </is>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" s="2" t="inlineStr">
-        <is>
-          <t>conv2 (Sequential)</t>
-        </is>
-      </c>
-      <c r="B9" s="2" t="inlineStr">
-        <is>
-          <t>(1, 16, 32, 32)</t>
-        </is>
-      </c>
-      <c r="C9" s="2" t="inlineStr">
-        <is>
-          <t>(1, 32, 16, 16)</t>
-        </is>
-      </c>
-      <c r="D9" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E9" s="2" t="n">
-        <v>96</v>
-      </c>
-      <c r="F9" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="G9" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="H9" s="2" t="inlineStr">
-        <is>
-          <t>Memory-bound ❗</t>
-        </is>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" s="1" t="inlineStr">
-        <is>
-          <t>conv3.cba_unit.0 (Conv2d)</t>
-        </is>
-      </c>
-      <c r="B10" s="1" t="inlineStr">
-        <is>
-          <t>(1, 32, 16, 16)</t>
-        </is>
-      </c>
-      <c r="C10" s="1" t="inlineStr">
-        <is>
-          <t>(1, 64, 8, 8)</t>
-        </is>
-      </c>
-      <c r="D10" s="1" t="n">
-        <v>9.437184</v>
-      </c>
-      <c r="E10" s="1" t="n">
-        <v>120</v>
-      </c>
-      <c r="F10" s="1" t="n">
-        <v>76.8</v>
-      </c>
-      <c r="G10" s="1" t="n">
-        <v>18.432</v>
-      </c>
-      <c r="H10" s="1" t="inlineStr">
-        <is>
-          <t>Balanced</t>
-        </is>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" s="2" t="inlineStr">
-        <is>
-          <t>conv3.cba_unit.1 (BatchNorm2d)</t>
-        </is>
-      </c>
-      <c r="B11" s="2" t="inlineStr">
-        <is>
-          <t>(1, 64, 8, 8)</t>
-        </is>
-      </c>
-      <c r="C11" s="2" t="inlineStr">
-        <is>
-          <t>(1, 64, 8, 8)</t>
-        </is>
-      </c>
-      <c r="D11" s="2" t="n">
-        <v>0.008192</v>
-      </c>
-      <c r="E11" s="2" t="n">
-        <v>32.5</v>
-      </c>
-      <c r="F11" s="2" t="n">
-        <v>0.25</v>
-      </c>
-      <c r="G11" s="2" t="n">
-        <v>0.128</v>
-      </c>
-      <c r="H11" s="2" t="inlineStr">
-        <is>
-          <t>Memory-bound ❗</t>
-        </is>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" s="2" t="inlineStr">
-        <is>
-          <t>conv3.cba_unit.2 (LeakyReLU)</t>
-        </is>
-      </c>
-      <c r="B12" s="2" t="inlineStr">
-        <is>
-          <t>(1, 64, 8, 8)</t>
-        </is>
-      </c>
-      <c r="C12" s="2" t="inlineStr">
-        <is>
-          <t>(1, 64, 8, 8)</t>
-        </is>
-      </c>
-      <c r="D12" s="2" t="n">
-        <v>0.004096</v>
-      </c>
-      <c r="E12" s="2" t="n">
-        <v>32</v>
-      </c>
-      <c r="F12" s="2" t="n">
-        <v>0.12</v>
-      </c>
-      <c r="G12" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="H12" s="2" t="inlineStr">
-        <is>
-          <t>Memory-bound ❗</t>
-        </is>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" s="2" t="inlineStr">
-        <is>
-          <t>conv3.cba_unit (Sequential)</t>
-        </is>
-      </c>
-      <c r="B13" s="2" t="inlineStr">
-        <is>
-          <t>(1, 32, 16, 16)</t>
-        </is>
-      </c>
-      <c r="C13" s="2" t="inlineStr">
-        <is>
-          <t>(1, 64, 8, 8)</t>
-        </is>
-      </c>
-      <c r="D13" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E13" s="2" t="n">
-        <v>48</v>
-      </c>
-      <c r="F13" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="G13" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="H13" s="2" t="inlineStr">
-        <is>
-          <t>Memory-bound ❗</t>
-        </is>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" s="2" t="inlineStr">
-        <is>
-          <t>conv3 (CBA)</t>
-        </is>
-      </c>
-      <c r="B14" s="2" t="inlineStr">
-        <is>
-          <t>(1, 32, 16, 16)</t>
-        </is>
-      </c>
-      <c r="C14" s="2" t="inlineStr">
-        <is>
-          <t>(1, 64, 8, 8)</t>
-        </is>
-      </c>
-      <c r="D14" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E14" s="2" t="n">
-        <v>48</v>
-      </c>
-      <c r="F14" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="G14" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="H14" s="2" t="inlineStr">
-        <is>
-          <t>Memory-bound ❗</t>
-        </is>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" s="2" t="inlineStr">
-        <is>
-          <t>fc (Linear)</t>
-        </is>
-      </c>
-      <c r="B15" s="2" t="inlineStr">
-        <is>
-          <t>(1, 4096)</t>
-        </is>
-      </c>
-      <c r="C15" s="2" t="inlineStr">
-        <is>
-          <t>(1, 10)</t>
-        </is>
-      </c>
-      <c r="D15" s="2" t="n">
-        <v>0.08192000000000001</v>
-      </c>
-      <c r="E15" s="2" t="n">
-        <v>176.078125</v>
-      </c>
-      <c r="F15" s="2" t="n">
-        <v>0.45</v>
-      </c>
-      <c r="G15" s="2" t="n">
-        <v>40.97</v>
-      </c>
-      <c r="H15" s="2" t="inlineStr">
-        <is>
-          <t>Memory-bound ❗</t>
-        </is>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" s="2" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> (SimpleCNN)</t>
-        </is>
-      </c>
-      <c r="B16" s="2" t="inlineStr">
-        <is>
-          <t>(1, 3, 32, 32)</t>
-        </is>
-      </c>
-      <c r="C16" s="2" t="inlineStr">
-        <is>
-          <t>(1, 10)</t>
-        </is>
-      </c>
-      <c r="D16" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E16" s="2" t="n">
-        <v>12.0390625</v>
-      </c>
-      <c r="F16" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="G16" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="H16" s="2" t="inlineStr">
         <is>
           <t>Memory-bound ❗</t>
         </is>
@@ -1046,13 +740,13 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>12</v>
+        <v>3</v>
       </c>
       <c r="C2" t="n">
-        <v>0.167936</v>
+        <v>0.08192000000000001</v>
       </c>
       <c r="D2" t="n">
-        <v>41.194</v>
+        <v>40.97</v>
       </c>
     </row>
     <row r="3">
@@ -1095,10 +789,10 @@
       </c>
       <c r="B6" t="inlineStr"/>
       <c r="C6" t="n">
-        <v>0.01992704</v>
+        <v>0.019841024</v>
       </c>
       <c r="D6" t="n">
-        <v>0.06471399999999999</v>
+        <v>0.06449000000000001</v>
       </c>
     </row>
     <row r="7">
@@ -1108,7 +802,7 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>1.246072</v>
+        <v>0.561144</v>
       </c>
     </row>
   </sheetData>

</xml_diff>